<commit_message>
Tokens are now properly deleted in UserDataManager
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheets/database_input.xlsx
+++ b/src/test/resources/ExcelSheets/database_input.xlsx
@@ -7,16 +7,18 @@
     <workbookView xWindow="192" yWindow="108" windowWidth="12420" windowHeight="8232"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="NewUsers" sheetId="1" r:id="rId1"/>
+    <sheet name="UserTemplate" sheetId="4" r:id="rId2"/>
+    <sheet name="clshaps93" sheetId="2" r:id="rId3"/>
+    <sheet name="emshaps90" sheetId="3" r:id="rId4"/>
+    <sheet name="NewJobInfo" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -141,12 +143,6 @@
     <t>I'm carrying the will</t>
   </si>
   <si>
-    <t>02/03/2017</t>
-  </si>
-  <si>
-    <t>01/22/2017</t>
-  </si>
-  <si>
     <t>graduationDate</t>
   </si>
   <si>
@@ -154,6 +150,30 @@
   </si>
   <si>
     <t>01/06/2017</t>
+  </si>
+  <si>
+    <t>01/16/2017</t>
+  </si>
+  <si>
+    <t>01/17/2017</t>
+  </si>
+  <si>
+    <t>01/19/2017</t>
+  </si>
+  <si>
+    <t>01/18/2017</t>
+  </si>
+  <si>
+    <t>note2</t>
+  </si>
+  <si>
+    <t>note3</t>
+  </si>
+  <si>
+    <t>note4</t>
+  </si>
+  <si>
+    <t>note5</t>
   </si>
 </sst>
 </file>
@@ -197,10 +217,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
@@ -497,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -547,213 +572,94 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" t="s">
-        <v>13</v>
+      <c r="A9" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1" t="s">
+      <c r="A11" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+    <row r="12" spans="1:11">
+      <c r="A12" s="5" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -764,24 +670,450 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="26" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="26" width="20.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
weekdays can be successfully retrieved from excel sheet (Expected) and a web page (Actual).
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheets/database_input.xlsx
+++ b/src/test/resources/ExcelSheets/database_input.xlsx
@@ -9,16 +9,15 @@
   <sheets>
     <sheet name="NewUsers" sheetId="1" r:id="rId1"/>
     <sheet name="UserTemplate" sheetId="4" r:id="rId2"/>
-    <sheet name="clshaps93" sheetId="2" r:id="rId3"/>
-    <sheet name="emshaps90" sheetId="3" r:id="rId4"/>
-    <sheet name="NewJobInfo" sheetId="5" r:id="rId5"/>
+    <sheet name="emshaps90" sheetId="3" r:id="rId3"/>
+    <sheet name="NewJobInfo" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
   <si>
     <t>username</t>
   </si>
@@ -137,9 +136,6 @@
     <t>superAdmin</t>
   </si>
   <si>
-    <t>My name is Jonas</t>
-  </si>
-  <si>
     <t>I'm carrying the will</t>
   </si>
   <si>
@@ -164,16 +160,19 @@
     <t>01/18/2017</t>
   </si>
   <si>
-    <t>note2</t>
-  </si>
-  <si>
-    <t>note3</t>
-  </si>
-  <si>
     <t>note4</t>
   </si>
   <si>
     <t>note5</t>
+  </si>
+  <si>
+    <t>01/20/2017</t>
+  </si>
+  <si>
+    <t>everything is false</t>
+  </si>
+  <si>
+    <t>STOP</t>
   </si>
 </sst>
 </file>
@@ -525,7 +524,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -585,6 +584,9 @@
       <c r="C3" t="s">
         <v>32</v>
       </c>
+      <c r="D3" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" t="s">
@@ -596,6 +598,9 @@
       <c r="C4" t="s">
         <v>30</v>
       </c>
+      <c r="D4" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
@@ -607,6 +612,9 @@
       <c r="C5" t="s">
         <v>33</v>
       </c>
+      <c r="D5" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -618,6 +626,9 @@
       <c r="C6" t="s">
         <v>35</v>
       </c>
+      <c r="D6" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
@@ -629,6 +640,9 @@
       <c r="C7" t="s">
         <v>37</v>
       </c>
+      <c r="D7" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
@@ -640,16 +654,22 @@
       <c r="C8" t="s">
         <v>21</v>
       </c>
+      <c r="D8" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>43</v>
+      <c r="D9" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -775,133 +795,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -910,9 +807,13 @@
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" customWidth="1"/>
     <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:9">
       <c r="A1" s="7" t="s">
         <v>28</v>
       </c>
@@ -931,27 +832,45 @@
       <c r="F1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -964,8 +883,17 @@
       <c r="D4" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -978,37 +906,52 @@
       <c r="D5" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="G6" s="7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1018,7 +961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J12"/>
   <sheetViews>

</xml_diff>

<commit_message>
Associate Tasks can now be initialized in the database.
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheets/database_input.xlsx
+++ b/src/test/resources/ExcelSheets/database_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="108" windowWidth="12420" windowHeight="8232"/>
+    <workbookView xWindow="192" yWindow="108" windowWidth="12420" windowHeight="8232" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewUsers" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
   <si>
     <t>username</t>
   </si>
@@ -161,6 +161,24 @@
   </si>
   <si>
     <t>STOP</t>
+  </si>
+  <si>
+    <t>02/08/2017</t>
+  </si>
+  <si>
+    <t>02/14/2017</t>
+  </si>
+  <si>
+    <t>Everything you want</t>
+  </si>
+  <si>
+    <t>Everything you need</t>
+  </si>
+  <si>
+    <t>Certification</t>
+  </si>
+  <si>
+    <t>Panel</t>
   </si>
 </sst>
 </file>
@@ -511,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -783,17 +801,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.5546875" customWidth="1"/>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.77734375" customWidth="1"/>
     <col min="4" max="4" width="11.109375" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="15.6640625" customWidth="1"/>
@@ -930,18 +948,78 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="B9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="B10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" t="s">
+      <c r="A11" s="7" t="s">
         <v>15</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -954,7 +1032,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
Changed test classes that interact with the database to reflect the new object types added to the database
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelSheets/database_input.xlsx
+++ b/src/test/resources/ExcelSheets/database_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="108" windowWidth="12420" windowHeight="8232" activeTab="2"/>
+    <workbookView xWindow="192" yWindow="108" windowWidth="12420" windowHeight="8232"/>
   </bookViews>
   <sheets>
     <sheet name="NewUsers" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
   <si>
     <t>username</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>Panel</t>
+  </si>
+  <si>
+    <t>marketingStatus</t>
   </si>
 </sst>
 </file>
@@ -527,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -678,13 +681,27 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="6" t="s">
+    <row r="10" spans="1:11">
+      <c r="A10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
     </row>
@@ -803,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>